<commit_message>
Updated Parser.java, Parsing Table.xlsx. Made Parsing Table readable. Tried to code reduce() but utterly failed in the end because fukkin productions are confusing as fuk.
</commit_message>
<xml_diff>
--- a/src/tweetspeak/resources/Parsing Table.xlsx
+++ b/src/tweetspeak/resources/Parsing Table.xlsx
@@ -1403,9 +1403,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1418,10 +1415,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1697,7 +1697,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1708,13 +1708,13 @@
   <dimension ref="A1:DD174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B15" sqref="B15"/>
+      <pane xSplit="1" topLeftCell="AR1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BF10" sqref="BF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -1874,384 +1874,384 @@
       <c r="BD1" s="7"/>
       <c r="BE1" s="7"/>
       <c r="BF1" s="7"/>
-      <c r="BG1" s="2" t="s">
+      <c r="BG1" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="BH1" s="2"/>
-      <c r="BI1" s="2"/>
-      <c r="BJ1" s="2"/>
-      <c r="BK1" s="2"/>
-      <c r="BL1" s="2"/>
-      <c r="BM1" s="2"/>
-      <c r="BN1" s="2"/>
-      <c r="BO1" s="2"/>
-      <c r="BP1" s="2"/>
-      <c r="BQ1" s="2"/>
-      <c r="BR1" s="2"/>
-      <c r="BS1" s="2"/>
-      <c r="BT1" s="2"/>
-      <c r="BU1" s="2"/>
-      <c r="BV1" s="2"/>
-      <c r="BW1" s="2"/>
-      <c r="BX1" s="2"/>
-      <c r="BY1" s="2"/>
-      <c r="BZ1" s="2"/>
-      <c r="CA1" s="2"/>
-      <c r="CB1" s="2"/>
-      <c r="CC1" s="2"/>
-      <c r="CD1" s="2"/>
-      <c r="CE1" s="2"/>
-      <c r="CF1" s="2"/>
-      <c r="CG1" s="2"/>
-      <c r="CH1" s="2"/>
-      <c r="CI1" s="2"/>
-      <c r="CJ1" s="2"/>
-      <c r="CK1" s="2"/>
-      <c r="CL1" s="2"/>
-      <c r="CM1" s="2"/>
-      <c r="CN1" s="2"/>
-      <c r="CO1" s="2"/>
-      <c r="CP1" s="2"/>
-      <c r="CQ1" s="2"/>
-      <c r="CR1" s="2"/>
-      <c r="CS1" s="2"/>
-      <c r="CT1" s="2"/>
-      <c r="CU1" s="2"/>
-      <c r="CV1" s="2"/>
-      <c r="CW1" s="2"/>
-      <c r="CX1" s="2"/>
-      <c r="CY1" s="2"/>
-      <c r="CZ1" s="2"/>
-      <c r="DA1" s="2"/>
-      <c r="DB1" s="2"/>
-      <c r="DC1" s="2"/>
-      <c r="DD1" s="2"/>
+      <c r="BH1" s="8"/>
+      <c r="BI1" s="8"/>
+      <c r="BJ1" s="8"/>
+      <c r="BK1" s="8"/>
+      <c r="BL1" s="8"/>
+      <c r="BM1" s="8"/>
+      <c r="BN1" s="8"/>
+      <c r="BO1" s="8"/>
+      <c r="BP1" s="8"/>
+      <c r="BQ1" s="8"/>
+      <c r="BR1" s="8"/>
+      <c r="BS1" s="8"/>
+      <c r="BT1" s="8"/>
+      <c r="BU1" s="8"/>
+      <c r="BV1" s="8"/>
+      <c r="BW1" s="8"/>
+      <c r="BX1" s="8"/>
+      <c r="BY1" s="8"/>
+      <c r="BZ1" s="8"/>
+      <c r="CA1" s="8"/>
+      <c r="CB1" s="8"/>
+      <c r="CC1" s="8"/>
+      <c r="CD1" s="8"/>
+      <c r="CE1" s="8"/>
+      <c r="CF1" s="8"/>
+      <c r="CG1" s="8"/>
+      <c r="CH1" s="8"/>
+      <c r="CI1" s="8"/>
+      <c r="CJ1" s="8"/>
+      <c r="CK1" s="8"/>
+      <c r="CL1" s="8"/>
+      <c r="CM1" s="8"/>
+      <c r="CN1" s="8"/>
+      <c r="CO1" s="8"/>
+      <c r="CP1" s="8"/>
+      <c r="CQ1" s="8"/>
+      <c r="CR1" s="8"/>
+      <c r="CS1" s="8"/>
+      <c r="CT1" s="8"/>
+      <c r="CU1" s="8"/>
+      <c r="CV1" s="8"/>
+      <c r="CW1" s="8"/>
+      <c r="CX1" s="8"/>
+      <c r="CY1" s="8"/>
+      <c r="CZ1" s="8"/>
+      <c r="DA1" s="8"/>
+      <c r="DB1" s="8"/>
+      <c r="DC1" s="8"/>
+      <c r="DD1" s="8"/>
     </row>
     <row r="2" spans="1:108">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="6" t="s">
+      <c r="S2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="6" t="s">
+      <c r="U2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="6" t="s">
+      <c r="W2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="X2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Y2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="Z2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AA2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AB2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AC2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AD2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="6" t="s">
+      <c r="AE2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AF2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AG2" s="6" t="s">
+      <c r="AG2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AH2" s="6" t="s">
+      <c r="AH2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AI2" s="6" t="s">
+      <c r="AI2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="AJ2" s="6" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AK2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AL2" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="AM2" s="6" t="s">
+      <c r="AM2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AN2" s="6" t="s">
+      <c r="AN2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AO2" s="6" t="s">
+      <c r="AO2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AP2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AQ2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AR2" s="6" t="s">
+      <c r="AR2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="AS2" s="6" t="s">
+      <c r="AS2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AT2" s="6" t="s">
+      <c r="AT2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="AU2" s="6" t="s">
+      <c r="AU2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AV2" s="6" t="s">
+      <c r="AV2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="AW2" s="6" t="s">
+      <c r="AW2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AX2" s="6" t="s">
+      <c r="AX2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AY2" s="6" t="s">
+      <c r="AY2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AZ2" s="6" t="s">
+      <c r="AZ2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="BA2" s="6" t="s">
+      <c r="BA2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="BB2" s="6" t="s">
+      <c r="BB2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="BC2" s="6" t="s">
+      <c r="BC2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="BD2" s="6" t="s">
+      <c r="BD2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="BE2" s="6" t="s">
+      <c r="BE2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="BF2" s="6" t="s">
+      <c r="BF2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="BG2" s="8" t="s">
+      <c r="BG2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="BH2" s="8" t="s">
+      <c r="BH2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="BI2" s="8" t="s">
+      <c r="BI2" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="BJ2" s="8" t="s">
+      <c r="BJ2" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="BK2" s="8" t="s">
+      <c r="BK2" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="BL2" s="8" t="s">
+      <c r="BL2" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="BM2" s="8" t="s">
+      <c r="BM2" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="BN2" s="8" t="s">
+      <c r="BN2" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="BO2" s="8" t="s">
+      <c r="BO2" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="BP2" s="8" t="s">
+      <c r="BP2" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="BQ2" s="8" t="s">
+      <c r="BQ2" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="BR2" s="8" t="s">
+      <c r="BR2" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="BS2" s="8" t="s">
+      <c r="BS2" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="BT2" s="8" t="s">
+      <c r="BT2" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="BU2" s="8" t="s">
+      <c r="BU2" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="BV2" s="8" t="s">
+      <c r="BV2" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="BW2" s="8" t="s">
+      <c r="BW2" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="BX2" s="8" t="s">
+      <c r="BX2" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="BY2" s="8" t="s">
+      <c r="BY2" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="BZ2" s="8" t="s">
+      <c r="BZ2" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="CA2" s="8" t="s">
+      <c r="CA2" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="CB2" s="8" t="s">
+      <c r="CB2" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="CC2" s="8" t="s">
+      <c r="CC2" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="CD2" s="8" t="s">
+      <c r="CD2" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="CE2" s="8" t="s">
+      <c r="CE2" s="6" t="s">
         <v>218</v>
       </c>
-      <c r="CF2" s="8" t="s">
+      <c r="CF2" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="CG2" s="8" t="s">
+      <c r="CG2" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="CH2" s="8" t="s">
+      <c r="CH2" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="CI2" s="8" t="s">
+      <c r="CI2" s="6" t="s">
         <v>222</v>
       </c>
-      <c r="CJ2" s="8" t="s">
+      <c r="CJ2" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="CK2" s="8" t="s">
+      <c r="CK2" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="CL2" s="8" t="s">
+      <c r="CL2" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="CM2" s="8" t="s">
+      <c r="CM2" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="CN2" s="8" t="s">
+      <c r="CN2" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="CO2" s="8" t="s">
+      <c r="CO2" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="CP2" s="8" t="s">
+      <c r="CP2" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="CQ2" s="8" t="s">
+      <c r="CQ2" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="CR2" s="8" t="s">
+      <c r="CR2" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="CS2" s="8" t="s">
+      <c r="CS2" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="CT2" s="8" t="s">
+      <c r="CT2" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="CU2" s="8" t="s">
+      <c r="CU2" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="CV2" s="8" t="s">
+      <c r="CV2" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="CW2" s="8" t="s">
+      <c r="CW2" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="CX2" s="8" t="s">
+      <c r="CX2" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="CY2" s="8" t="s">
+      <c r="CY2" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="CZ2" s="8" t="s">
+      <c r="CZ2" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="DA2" s="8" t="s">
+      <c r="DA2" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="DB2" s="8" t="s">
+      <c r="DB2" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="DC2" s="8" t="s">
+      <c r="DC2" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="DD2" s="8" t="s">
+      <c r="DD2" s="6" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:108">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>70</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -2262,15 +2262,15 @@
       </c>
     </row>
     <row r="4" spans="1:108">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="BF4" s="3" t="s">
+      <c r="BF4" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:108">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>56</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2278,7 +2278,7 @@
       </c>
     </row>
     <row r="6" spans="1:108">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -2286,7 +2286,7 @@
       </c>
     </row>
     <row r="7" spans="1:108">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -2300,7 +2300,7 @@
       </c>
     </row>
     <row r="8" spans="1:108">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>59</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -2308,7 +2308,7 @@
       </c>
     </row>
     <row r="9" spans="1:108">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>60</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="10" spans="1:108">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>61</v>
       </c>
       <c r="BF10" s="1" t="s">
@@ -2324,7 +2324,7 @@
       </c>
     </row>
     <row r="11" spans="1:108">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -2353,7 +2353,7 @@
       </c>
     </row>
     <row r="12" spans="1:108">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>63</v>
       </c>
       <c r="E12" s="1" t="s">
@@ -2361,7 +2361,7 @@
       </c>
     </row>
     <row r="13" spans="1:108">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>64</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -2369,7 +2369,7 @@
       </c>
     </row>
     <row r="14" spans="1:108">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>65</v>
       </c>
       <c r="N14" s="1" t="s">
@@ -2485,7 +2485,7 @@
       </c>
     </row>
     <row r="15" spans="1:108">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2547,7 +2547,7 @@
       </c>
     </row>
     <row r="16" spans="1:108">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>67</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -2609,7 +2609,7 @@
       </c>
     </row>
     <row r="17" spans="1:50">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>68</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -2671,7 +2671,7 @@
       </c>
     </row>
     <row r="18" spans="1:50">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>69</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2733,7 +2733,7 @@
       </c>
     </row>
     <row r="19" spans="1:50">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>80</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -2795,7 +2795,7 @@
       </c>
     </row>
     <row r="20" spans="1:50">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>81</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -2857,7 +2857,7 @@
       </c>
     </row>
     <row r="21" spans="1:50">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>82</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -2919,7 +2919,7 @@
       </c>
     </row>
     <row r="22" spans="1:50">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>83</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -2981,7 +2981,7 @@
       </c>
     </row>
     <row r="23" spans="1:50">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>84</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -3043,7 +3043,7 @@
       </c>
     </row>
     <row r="24" spans="1:50">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>85</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -3105,7 +3105,7 @@
       </c>
     </row>
     <row r="25" spans="1:50">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>86</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -3167,7 +3167,7 @@
       </c>
     </row>
     <row r="26" spans="1:50">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -3229,7 +3229,7 @@
       </c>
     </row>
     <row r="27" spans="1:50">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -3291,7 +3291,7 @@
       </c>
     </row>
     <row r="28" spans="1:50">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>89</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -3353,7 +3353,7 @@
       </c>
     </row>
     <row r="29" spans="1:50">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -3415,7 +3415,7 @@
       </c>
     </row>
     <row r="30" spans="1:50">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -3474,7 +3474,7 @@
       </c>
     </row>
     <row r="31" spans="1:50">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -3533,7 +3533,7 @@
       </c>
     </row>
     <row r="32" spans="1:50">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>93</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -3592,7 +3592,7 @@
       </c>
     </row>
     <row r="33" spans="1:108">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>94</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -3651,7 +3651,7 @@
       </c>
     </row>
     <row r="34" spans="1:108">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>95</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -3710,7 +3710,7 @@
       </c>
     </row>
     <row r="35" spans="1:108">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -3769,7 +3769,7 @@
       </c>
     </row>
     <row r="36" spans="1:108">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="5" t="s">
         <v>97</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -3831,7 +3831,7 @@
       </c>
     </row>
     <row r="37" spans="1:108">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="5" t="s">
         <v>98</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -3893,7 +3893,7 @@
       </c>
     </row>
     <row r="38" spans="1:108">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>99</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -3955,7 +3955,7 @@
       </c>
     </row>
     <row r="39" spans="1:108">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>100</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -4017,7 +4017,7 @@
       </c>
     </row>
     <row r="40" spans="1:108">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>101</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -4079,7 +4079,7 @@
       </c>
     </row>
     <row r="41" spans="1:108">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>102</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -4141,7 +4141,7 @@
       </c>
     </row>
     <row r="42" spans="1:108">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
         <v>103</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -4203,7 +4203,7 @@
       </c>
     </row>
     <row r="43" spans="1:108">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -4265,7 +4265,7 @@
       </c>
     </row>
     <row r="44" spans="1:108">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="5" t="s">
         <v>105</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -4327,7 +4327,7 @@
       </c>
     </row>
     <row r="45" spans="1:108">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="5" t="s">
         <v>106</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -4335,7 +4335,7 @@
       </c>
     </row>
     <row r="46" spans="1:108">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="5" t="s">
         <v>107</v>
       </c>
       <c r="E46" s="1" t="s">
@@ -4400,7 +4400,7 @@
       </c>
     </row>
     <row r="47" spans="1:108">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="5" t="s">
         <v>108</v>
       </c>
       <c r="AY47" s="1" t="s">
@@ -4432,7 +4432,7 @@
       </c>
     </row>
     <row r="48" spans="1:108">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="5" t="s">
         <v>109</v>
       </c>
       <c r="E48" s="1" t="s">
@@ -4494,7 +4494,7 @@
       </c>
     </row>
     <row r="49" spans="1:107">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="5" t="s">
         <v>110</v>
       </c>
       <c r="E49" s="1" t="s">
@@ -4559,7 +4559,7 @@
       </c>
     </row>
     <row r="50" spans="1:107">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="5" t="s">
         <v>111</v>
       </c>
       <c r="E50" s="1" t="s">
@@ -4624,7 +4624,7 @@
       </c>
     </row>
     <row r="51" spans="1:107">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="5" t="s">
         <v>112</v>
       </c>
       <c r="E51" s="1" t="s">
@@ -4689,7 +4689,7 @@
       </c>
     </row>
     <row r="52" spans="1:107">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="5" t="s">
         <v>113</v>
       </c>
       <c r="E52" s="1" t="s">
@@ -4754,7 +4754,7 @@
       </c>
     </row>
     <row r="53" spans="1:107">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="5" t="s">
         <v>114</v>
       </c>
       <c r="E53" s="1" t="s">
@@ -4819,7 +4819,7 @@
       </c>
     </row>
     <row r="54" spans="1:107">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="5" t="s">
         <v>115</v>
       </c>
       <c r="E54" s="1" t="s">
@@ -4884,7 +4884,7 @@
       </c>
     </row>
     <row r="55" spans="1:107">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="5" t="s">
         <v>116</v>
       </c>
       <c r="E55" s="1" t="s">
@@ -4949,7 +4949,7 @@
       </c>
     </row>
     <row r="56" spans="1:107">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="5" t="s">
         <v>117</v>
       </c>
       <c r="E56" s="1" t="s">
@@ -5014,7 +5014,7 @@
       </c>
     </row>
     <row r="57" spans="1:107">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="5" t="s">
         <v>118</v>
       </c>
       <c r="C57" s="1" t="s">
@@ -5022,7 +5022,7 @@
       </c>
     </row>
     <row r="58" spans="1:107">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="5" t="s">
         <v>119</v>
       </c>
       <c r="C58" s="1" t="s">
@@ -5082,7 +5082,7 @@
       <c r="CW58" s="1">
         <v>123</v>
       </c>
-      <c r="DB58" s="4" t="s">
+      <c r="DB58" s="3" t="s">
         <v>359</v>
       </c>
       <c r="DC58" s="1">
@@ -5090,12 +5090,12 @@
       </c>
     </row>
     <row r="59" spans="1:107">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:107">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="5" t="s">
         <v>121</v>
       </c>
       <c r="E60" s="1" t="s">
@@ -5163,12 +5163,12 @@
       </c>
     </row>
     <row r="61" spans="1:107">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="5" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:107">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="5" t="s">
         <v>123</v>
       </c>
       <c r="AM62" s="1" t="s">
@@ -5176,7 +5176,7 @@
       </c>
     </row>
     <row r="63" spans="1:107">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="5" t="s">
         <v>124</v>
       </c>
       <c r="C63" s="1" t="s">
@@ -5184,7 +5184,7 @@
       </c>
     </row>
     <row r="64" spans="1:107">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="5" t="s">
         <v>125</v>
       </c>
       <c r="H64" s="1" t="s">
@@ -5192,7 +5192,7 @@
       </c>
     </row>
     <row r="65" spans="1:94">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="5" t="s">
         <v>126</v>
       </c>
       <c r="CC65" s="1">
@@ -5200,7 +5200,7 @@
       </c>
     </row>
     <row r="66" spans="1:94">
-      <c r="A66" s="6" t="s">
+      <c r="A66" s="5" t="s">
         <v>127</v>
       </c>
       <c r="I66" s="1" t="s">
@@ -5208,7 +5208,7 @@
       </c>
     </row>
     <row r="67" spans="1:94">
-      <c r="A67" s="6" t="s">
+      <c r="A67" s="5" t="s">
         <v>128</v>
       </c>
       <c r="E67" s="1" t="s">
@@ -5270,27 +5270,27 @@
       </c>
     </row>
     <row r="68" spans="1:94">
-      <c r="A68" s="6" t="s">
+      <c r="A68" s="5" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="69" spans="1:94">
-      <c r="A69" s="6" t="s">
+      <c r="A69" s="5" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="70" spans="1:94">
-      <c r="A70" s="6" t="s">
+      <c r="A70" s="5" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="71" spans="1:94">
-      <c r="A71" s="6" t="s">
+      <c r="A71" s="5" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="72" spans="1:94">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="5" t="s">
         <v>133</v>
       </c>
       <c r="CO72" s="1">
@@ -5298,7 +5298,7 @@
       </c>
     </row>
     <row r="73" spans="1:94">
-      <c r="A73" s="6" t="s">
+      <c r="A73" s="5" t="s">
         <v>134</v>
       </c>
       <c r="CO73" s="1">
@@ -5306,27 +5306,27 @@
       </c>
     </row>
     <row r="74" spans="1:94">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="5" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="75" spans="1:94">
-      <c r="A75" s="6" t="s">
+      <c r="A75" s="5" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:94">
-      <c r="A76" s="6" t="s">
+      <c r="A76" s="5" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="77" spans="1:94">
-      <c r="A77" s="6" t="s">
+      <c r="A77" s="5" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="78" spans="1:94">
-      <c r="A78" s="6" t="s">
+      <c r="A78" s="5" t="s">
         <v>139</v>
       </c>
       <c r="E78" s="1" t="s">
@@ -5397,7 +5397,7 @@
       </c>
     </row>
     <row r="79" spans="1:94">
-      <c r="A79" s="6" t="s">
+      <c r="A79" s="5" t="s">
         <v>140</v>
       </c>
       <c r="CP79" s="1">
@@ -5405,7 +5405,7 @@
       </c>
     </row>
     <row r="80" spans="1:94">
-      <c r="A80" s="6" t="s">
+      <c r="A80" s="5" t="s">
         <v>141</v>
       </c>
       <c r="CP80" s="1">
@@ -5413,7 +5413,7 @@
       </c>
     </row>
     <row r="81" spans="1:96">
-      <c r="A81" s="6" t="s">
+      <c r="A81" s="5" t="s">
         <v>142</v>
       </c>
       <c r="CP81" s="1">
@@ -5421,7 +5421,7 @@
       </c>
     </row>
     <row r="82" spans="1:96">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="5" t="s">
         <v>143</v>
       </c>
       <c r="E82" s="1" t="s">
@@ -5483,7 +5483,7 @@
       </c>
     </row>
     <row r="83" spans="1:96">
-      <c r="A83" s="6" t="s">
+      <c r="A83" s="5" t="s">
         <v>144</v>
       </c>
       <c r="E83" s="1" t="s">
@@ -5545,7 +5545,7 @@
       </c>
     </row>
     <row r="84" spans="1:96">
-      <c r="A84" s="6" t="s">
+      <c r="A84" s="5" t="s">
         <v>145</v>
       </c>
       <c r="E84" s="1" t="s">
@@ -5607,22 +5607,22 @@
       </c>
     </row>
     <row r="85" spans="1:96">
-      <c r="A85" s="6" t="s">
+      <c r="A85" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="86" spans="1:96">
-      <c r="A86" s="6" t="s">
+      <c r="A86" s="5" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="87" spans="1:96">
-      <c r="A87" s="6" t="s">
+      <c r="A87" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="88" spans="1:96">
-      <c r="A88" s="6" t="s">
+      <c r="A88" s="5" t="s">
         <v>149</v>
       </c>
       <c r="E88" s="1" t="s">
@@ -5687,7 +5687,7 @@
       </c>
     </row>
     <row r="89" spans="1:96">
-      <c r="A89" s="6" t="s">
+      <c r="A89" s="5" t="s">
         <v>150</v>
       </c>
       <c r="CR89" s="1">
@@ -5695,7 +5695,7 @@
       </c>
     </row>
     <row r="90" spans="1:96">
-      <c r="A90" s="6" t="s">
+      <c r="A90" s="5" t="s">
         <v>151</v>
       </c>
       <c r="E90" s="1" t="s">
@@ -5757,62 +5757,62 @@
       </c>
     </row>
     <row r="91" spans="1:96">
-      <c r="A91" s="6" t="s">
+      <c r="A91" s="5" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="92" spans="1:96">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="93" spans="1:96">
-      <c r="A93" s="6" t="s">
+      <c r="A93" s="5" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="94" spans="1:96">
-      <c r="A94" s="6" t="s">
+      <c r="A94" s="5" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="95" spans="1:96">
-      <c r="A95" s="6" t="s">
+      <c r="A95" s="5" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="96" spans="1:96">
-      <c r="A96" s="6" t="s">
+      <c r="A96" s="5" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="97" spans="1:100">
-      <c r="A97" s="6" t="s">
+      <c r="A97" s="5" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="98" spans="1:100">
-      <c r="A98" s="6" t="s">
+      <c r="A98" s="5" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="99" spans="1:100">
-      <c r="A99" s="6" t="s">
+      <c r="A99" s="5" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="100" spans="1:100">
-      <c r="A100" s="6" t="s">
+      <c r="A100" s="5" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="101" spans="1:100">
-      <c r="A101" s="6" t="s">
+      <c r="A101" s="5" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="102" spans="1:100">
-      <c r="A102" s="6" t="s">
+      <c r="A102" s="5" t="s">
         <v>163</v>
       </c>
       <c r="CS102" s="1">
@@ -5820,7 +5820,7 @@
       </c>
     </row>
     <row r="103" spans="1:100">
-      <c r="A103" s="6" t="s">
+      <c r="A103" s="5" t="s">
         <v>164</v>
       </c>
       <c r="E103" s="1" t="s">
@@ -5882,7 +5882,7 @@
       </c>
     </row>
     <row r="104" spans="1:100">
-      <c r="A104" s="6" t="s">
+      <c r="A104" s="5" t="s">
         <v>165</v>
       </c>
       <c r="E104" s="1" t="s">
@@ -5947,7 +5947,7 @@
       </c>
     </row>
     <row r="105" spans="1:100">
-      <c r="A105" s="6" t="s">
+      <c r="A105" s="5" t="s">
         <v>166</v>
       </c>
       <c r="CU105" s="1">
@@ -5955,7 +5955,7 @@
       </c>
     </row>
     <row r="106" spans="1:100">
-      <c r="A106" s="6" t="s">
+      <c r="A106" s="5" t="s">
         <v>167</v>
       </c>
       <c r="AO106" s="1" t="s">
@@ -5963,7 +5963,7 @@
       </c>
     </row>
     <row r="107" spans="1:100">
-      <c r="A107" s="6" t="s">
+      <c r="A107" s="5" t="s">
         <v>168</v>
       </c>
       <c r="CV107" s="1">
@@ -5971,7 +5971,7 @@
       </c>
     </row>
     <row r="108" spans="1:100">
-      <c r="A108" s="6" t="s">
+      <c r="A108" s="5" t="s">
         <v>169</v>
       </c>
       <c r="E108" s="1" t="s">
@@ -6033,7 +6033,7 @@
       </c>
     </row>
     <row r="109" spans="1:100">
-      <c r="A109" s="6" t="s">
+      <c r="A109" s="5" t="s">
         <v>170</v>
       </c>
       <c r="AP109" s="1" t="s">
@@ -6041,7 +6041,7 @@
       </c>
     </row>
     <row r="110" spans="1:100">
-      <c r="A110" s="6" t="s">
+      <c r="A110" s="5" t="s">
         <v>171</v>
       </c>
       <c r="CV110" s="1">
@@ -6049,7 +6049,7 @@
       </c>
     </row>
     <row r="111" spans="1:100">
-      <c r="A111" s="6" t="s">
+      <c r="A111" s="5" t="s">
         <v>172</v>
       </c>
       <c r="E111" s="1" t="s">
@@ -6111,7 +6111,7 @@
       </c>
     </row>
     <row r="112" spans="1:100">
-      <c r="A112" s="6" t="s">
+      <c r="A112" s="5" t="s">
         <v>173</v>
       </c>
       <c r="E112" s="1" t="s">
@@ -6173,7 +6173,7 @@
       </c>
     </row>
     <row r="113" spans="1:101">
-      <c r="A113" s="6" t="s">
+      <c r="A113" s="5" t="s">
         <v>174</v>
       </c>
       <c r="AQ113" s="1" t="s">
@@ -6181,7 +6181,7 @@
       </c>
     </row>
     <row r="114" spans="1:101">
-      <c r="A114" s="6" t="s">
+      <c r="A114" s="5" t="s">
         <v>175</v>
       </c>
       <c r="CW114" s="1">
@@ -6189,7 +6189,7 @@
       </c>
     </row>
     <row r="115" spans="1:101">
-      <c r="A115" s="6" t="s">
+      <c r="A115" s="5" t="s">
         <v>176</v>
       </c>
       <c r="E115" s="1" t="s">
@@ -6251,7 +6251,7 @@
       </c>
     </row>
     <row r="116" spans="1:101">
-      <c r="A116" s="6" t="s">
+      <c r="A116" s="5" t="s">
         <v>177</v>
       </c>
       <c r="AR116" s="1" t="s">
@@ -6259,7 +6259,7 @@
       </c>
     </row>
     <row r="117" spans="1:101">
-      <c r="A117" s="6" t="s">
+      <c r="A117" s="5" t="s">
         <v>178</v>
       </c>
       <c r="CW117" s="1">
@@ -6267,7 +6267,7 @@
       </c>
     </row>
     <row r="118" spans="1:101">
-      <c r="A118" s="6" t="s">
+      <c r="A118" s="5" t="s">
         <v>179</v>
       </c>
       <c r="E118" s="1" t="s">
@@ -6329,7 +6329,7 @@
       </c>
     </row>
     <row r="119" spans="1:101">
-      <c r="A119" s="6" t="s">
+      <c r="A119" s="5" t="s">
         <v>180</v>
       </c>
       <c r="AT119" s="1" t="s">
@@ -6337,7 +6337,7 @@
       </c>
     </row>
     <row r="120" spans="1:101">
-      <c r="A120" s="6" t="s">
+      <c r="A120" s="5" t="s">
         <v>181</v>
       </c>
       <c r="CW120" s="1">
@@ -6345,7 +6345,7 @@
       </c>
     </row>
     <row r="121" spans="1:101">
-      <c r="A121" s="6" t="s">
+      <c r="A121" s="5" t="s">
         <v>182</v>
       </c>
       <c r="E121" s="1" t="s">
@@ -6407,7 +6407,7 @@
       </c>
     </row>
     <row r="122" spans="1:101">
-      <c r="A122" s="6" t="s">
+      <c r="A122" s="5" t="s">
         <v>183</v>
       </c>
       <c r="AU122" s="1" t="s">
@@ -6415,7 +6415,7 @@
       </c>
     </row>
     <row r="123" spans="1:101">
-      <c r="A123" s="6" t="s">
+      <c r="A123" s="5" t="s">
         <v>184</v>
       </c>
       <c r="CW123" s="1">
@@ -6423,7 +6423,7 @@
       </c>
     </row>
     <row r="124" spans="1:101">
-      <c r="A124" s="6" t="s">
+      <c r="A124" s="5" t="s">
         <v>185</v>
       </c>
       <c r="E124" s="1" t="s">
@@ -6485,7 +6485,7 @@
       </c>
     </row>
     <row r="125" spans="1:101">
-      <c r="A125" s="6" t="s">
+      <c r="A125" s="5" t="s">
         <v>186</v>
       </c>
       <c r="E125" s="1" t="s">
@@ -6547,7 +6547,7 @@
       </c>
     </row>
     <row r="126" spans="1:101">
-      <c r="A126" s="6" t="s">
+      <c r="A126" s="5" t="s">
         <v>187</v>
       </c>
       <c r="CS126" s="1">
@@ -6555,7 +6555,7 @@
       </c>
     </row>
     <row r="127" spans="1:101">
-      <c r="A127" s="6" t="s">
+      <c r="A127" s="5" t="s">
         <v>188</v>
       </c>
       <c r="E127" s="1" t="s">
@@ -6617,7 +6617,7 @@
       </c>
     </row>
     <row r="128" spans="1:101">
-      <c r="A128" s="6" t="s">
+      <c r="A128" s="5" t="s">
         <v>189</v>
       </c>
       <c r="E128" s="1" t="s">
@@ -6679,7 +6679,7 @@
       </c>
     </row>
     <row r="129" spans="1:107">
-      <c r="A129" s="6" t="s">
+      <c r="A129" s="5" t="s">
         <v>190</v>
       </c>
       <c r="E129" s="1" t="s">
@@ -6741,7 +6741,7 @@
       </c>
     </row>
     <row r="130" spans="1:107">
-      <c r="A130" s="6" t="s">
+      <c r="A130" s="5" t="s">
         <v>191</v>
       </c>
       <c r="E130" s="1" t="s">
@@ -6803,7 +6803,7 @@
       </c>
     </row>
     <row r="131" spans="1:107">
-      <c r="A131" s="6" t="s">
+      <c r="A131" s="5" t="s">
         <v>192</v>
       </c>
       <c r="C131" s="1" t="s">
@@ -6811,7 +6811,7 @@
       </c>
     </row>
     <row r="132" spans="1:107">
-      <c r="A132" s="6" t="s">
+      <c r="A132" s="5" t="s">
         <v>193</v>
       </c>
       <c r="H132" s="1" t="s">
@@ -6819,7 +6819,7 @@
       </c>
     </row>
     <row r="133" spans="1:107">
-      <c r="A133" s="6" t="s">
+      <c r="A133" s="5" t="s">
         <v>194</v>
       </c>
       <c r="P133" s="1" t="s">
@@ -6827,7 +6827,7 @@
       </c>
     </row>
     <row r="134" spans="1:107">
-      <c r="A134" s="6" t="s">
+      <c r="A134" s="5" t="s">
         <v>195</v>
       </c>
       <c r="I134" s="1" t="s">
@@ -6835,7 +6835,7 @@
       </c>
     </row>
     <row r="135" spans="1:107">
-      <c r="A135" s="6" t="s">
+      <c r="A135" s="5" t="s">
         <v>360</v>
       </c>
       <c r="E135" s="1" t="s">
@@ -6897,37 +6897,37 @@
       </c>
     </row>
     <row r="136" spans="1:107">
-      <c r="A136" s="6" t="s">
+      <c r="A136" s="5" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="137" spans="1:107">
-      <c r="A137" s="6" t="s">
+      <c r="A137" s="5" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="138" spans="1:107">
-      <c r="A138" s="6" t="s">
+      <c r="A138" s="5" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="139" spans="1:107">
-      <c r="A139" s="6" t="s">
+      <c r="A139" s="5" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="140" spans="1:107">
-      <c r="A140" s="6" t="s">
+      <c r="A140" s="5" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="141" spans="1:107">
-      <c r="A141" s="6" t="s">
+      <c r="A141" s="5" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="142" spans="1:107">
-      <c r="A142" s="6" t="s">
+      <c r="A142" s="5" t="s">
         <v>367</v>
       </c>
       <c r="C142" s="1" t="s">
@@ -6987,7 +6987,7 @@
       <c r="CW142" s="1">
         <v>123</v>
       </c>
-      <c r="DB142" s="4" t="s">
+      <c r="DB142" s="3" t="s">
         <v>394</v>
       </c>
       <c r="DC142" s="1">
@@ -6995,7 +6995,7 @@
       </c>
     </row>
     <row r="143" spans="1:107">
-      <c r="A143" s="6" t="s">
+      <c r="A143" s="5" t="s">
         <v>368</v>
       </c>
       <c r="E143" s="1" t="s">
@@ -7057,7 +7057,7 @@
       </c>
     </row>
     <row r="144" spans="1:107">
-      <c r="A144" s="6" t="s">
+      <c r="A144" s="5" t="s">
         <v>369</v>
       </c>
       <c r="C144" s="1" t="s">
@@ -7065,7 +7065,7 @@
       </c>
     </row>
     <row r="145" spans="1:97">
-      <c r="A145" s="6" t="s">
+      <c r="A145" s="5" t="s">
         <v>370</v>
       </c>
       <c r="E145" s="1" t="s">
@@ -7127,7 +7127,7 @@
       </c>
     </row>
     <row r="146" spans="1:97">
-      <c r="A146" s="6" t="s">
+      <c r="A146" s="5" t="s">
         <v>371</v>
       </c>
       <c r="CB146" s="1">
@@ -7135,7 +7135,7 @@
       </c>
     </row>
     <row r="147" spans="1:97">
-      <c r="A147" s="6" t="s">
+      <c r="A147" s="5" t="s">
         <v>372</v>
       </c>
       <c r="E147" s="1" t="s">
@@ -7197,7 +7197,7 @@
       </c>
     </row>
     <row r="148" spans="1:97">
-      <c r="A148" s="6" t="s">
+      <c r="A148" s="5" t="s">
         <v>373</v>
       </c>
       <c r="H148" s="1" t="s">
@@ -7205,7 +7205,7 @@
       </c>
     </row>
     <row r="149" spans="1:97">
-      <c r="A149" s="6" t="s">
+      <c r="A149" s="5" t="s">
         <v>374</v>
       </c>
       <c r="CS149" s="1">
@@ -7213,7 +7213,7 @@
       </c>
     </row>
     <row r="150" spans="1:97">
-      <c r="A150" s="6" t="s">
+      <c r="A150" s="5" t="s">
         <v>375</v>
       </c>
       <c r="I150" s="1" t="s">
@@ -7224,7 +7224,7 @@
       </c>
     </row>
     <row r="151" spans="1:97">
-      <c r="A151" s="6" t="s">
+      <c r="A151" s="5" t="s">
         <v>376</v>
       </c>
       <c r="D151" s="1" t="s">
@@ -7232,15 +7232,15 @@
       </c>
     </row>
     <row r="152" spans="1:97">
-      <c r="A152" s="6" t="s">
+      <c r="A152" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="BM152" s="5">
+      <c r="BM152" s="4">
         <v>153</v>
       </c>
     </row>
     <row r="153" spans="1:97">
-      <c r="A153" s="6" t="s">
+      <c r="A153" s="5" t="s">
         <v>378</v>
       </c>
       <c r="E153" s="1" t="s">
@@ -7302,7 +7302,7 @@
       </c>
     </row>
     <row r="154" spans="1:97">
-      <c r="A154" s="6" t="s">
+      <c r="A154" s="5" t="s">
         <v>379</v>
       </c>
       <c r="E154" s="1" t="s">
@@ -7364,7 +7364,7 @@
       </c>
     </row>
     <row r="155" spans="1:97">
-      <c r="A155" s="6" t="s">
+      <c r="A155" s="5" t="s">
         <v>380</v>
       </c>
       <c r="E155" s="1" t="s">
@@ -7372,7 +7372,7 @@
       </c>
     </row>
     <row r="156" spans="1:97">
-      <c r="A156" s="6" t="s">
+      <c r="A156" s="5" t="s">
         <v>381</v>
       </c>
       <c r="E156" s="1" t="s">
@@ -7434,7 +7434,7 @@
       </c>
     </row>
     <row r="157" spans="1:97">
-      <c r="A157" s="6" t="s">
+      <c r="A157" s="5" t="s">
         <v>382</v>
       </c>
       <c r="H157" s="1" t="s">
@@ -7442,7 +7442,7 @@
       </c>
     </row>
     <row r="158" spans="1:97">
-      <c r="A158" s="6" t="s">
+      <c r="A158" s="5" t="s">
         <v>383</v>
       </c>
       <c r="CS158" s="1">
@@ -7450,7 +7450,7 @@
       </c>
     </row>
     <row r="159" spans="1:97">
-      <c r="A159" s="6" t="s">
+      <c r="A159" s="5" t="s">
         <v>384</v>
       </c>
       <c r="I159" s="1" t="s">
@@ -7458,7 +7458,7 @@
       </c>
     </row>
     <row r="160" spans="1:97">
-      <c r="A160" s="6" t="s">
+      <c r="A160" s="5" t="s">
         <v>385</v>
       </c>
       <c r="E160" s="1" t="s">
@@ -7466,7 +7466,7 @@
       </c>
     </row>
     <row r="161" spans="1:98">
-      <c r="A161" s="6" t="s">
+      <c r="A161" s="5" t="s">
         <v>386</v>
       </c>
       <c r="BM161" s="1">
@@ -7477,7 +7477,7 @@
       </c>
     </row>
     <row r="162" spans="1:98">
-      <c r="A162" s="6" t="s">
+      <c r="A162" s="5" t="s">
         <v>387</v>
       </c>
       <c r="E162" s="1" t="s">
@@ -7533,7 +7533,7 @@
       </c>
     </row>
     <row r="163" spans="1:98">
-      <c r="A163" s="6" t="s">
+      <c r="A163" s="5" t="s">
         <v>388</v>
       </c>
       <c r="E163" s="1" t="s">
@@ -7541,7 +7541,7 @@
       </c>
     </row>
     <row r="164" spans="1:98">
-      <c r="A164" s="6" t="s">
+      <c r="A164" s="5" t="s">
         <v>389</v>
       </c>
       <c r="E164" s="1" t="s">
@@ -7597,7 +7597,7 @@
       </c>
     </row>
     <row r="165" spans="1:98">
-      <c r="A165" s="6" t="s">
+      <c r="A165" s="5" t="s">
         <v>407</v>
       </c>
       <c r="CT165" s="1">
@@ -7605,47 +7605,47 @@
       </c>
     </row>
     <row r="166" spans="1:98">
-      <c r="A166" s="6" t="s">
+      <c r="A166" s="5" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="167" spans="1:98">
-      <c r="A167" s="6" t="s">
+      <c r="A167" s="5" t="s">
         <v>409</v>
       </c>
     </row>
     <row r="168" spans="1:98">
-      <c r="A168" s="6" t="s">
+      <c r="A168" s="5" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="169" spans="1:98">
-      <c r="A169" s="6" t="s">
+      <c r="A169" s="5" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="170" spans="1:98">
-      <c r="A170" s="6" t="s">
+      <c r="A170" s="5" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="171" spans="1:98">
-      <c r="A171" s="6" t="s">
+      <c r="A171" s="5" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="172" spans="1:98">
-      <c r="A172" s="6" t="s">
+      <c r="A172" s="5" t="s">
         <v>414</v>
       </c>
     </row>
     <row r="173" spans="1:98">
-      <c r="A173" s="6" t="s">
+      <c r="A173" s="5" t="s">
         <v>415</v>
       </c>
     </row>
     <row r="174" spans="1:98">
-      <c r="A174" s="6" t="s">
+      <c r="A174" s="5" t="s">
         <v>416</v>
       </c>
     </row>

</xml_diff>